<commit_message>
update CSS library 7/02
</commit_message>
<xml_diff>
--- a/CSS library.xlsx
+++ b/CSS library.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23175" windowHeight="9675"/>
+    <workbookView windowWidth="27795" windowHeight="12450" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$22</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -95,6 +96,76 @@
   </si>
   <si>
     <t>x y color blur;</t>
+  </si>
+  <si>
+    <t>font</t>
+  </si>
+  <si>
+    <t>Font-family</t>
+  </si>
+  <si>
+    <t>Font-face</t>
+  </si>
+  <si>
+    <t>Tự tạo tên font có trên máy của bạn</t>
+  </si>
+  <si>
+    <t>border</t>
+  </si>
+  <si>
+    <t>Border-width</t>
+  </si>
+  <si>
+    <t>Border-style</t>
+  </si>
+  <si>
+    <t>Border-color</t>
+  </si>
+  <si>
+    <t>Background-color</t>
+  </si>
+  <si>
+    <t>transparent</t>
+  </si>
+  <si>
+    <t>gradient</t>
+  </si>
+  <si>
+    <t>Background-image</t>
+  </si>
+  <si>
+    <t>abstract pattern</t>
+  </si>
+  <si>
+    <t>Repeat-x,repeat-y</t>
+  </si>
+  <si>
+    <t>Hình lặp đi lặp lại, mặc định lặp đi lặp lại, lặp lại theo trục x/y</t>
+  </si>
+  <si>
+    <t>Background-size</t>
+  </si>
+  <si>
+    <t>Cover : fixed hình, center : căn giữa hình</t>
+  </si>
+  <si>
+    <t>Background-position: 0px 1px</t>
+  </si>
+  <si>
+    <t>x,y</t>
+  </si>
+  <si>
+    <t>Background-attachment: fixed;</t>
+  </si>
+  <si>
+    <t>fix hình, hiệu ứng di chuyển</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>fontawesome.com
+material-design icon</t>
   </si>
 </sst>
 </file>
@@ -102,18 +173,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+  <fonts count="23">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -121,33 +191,18 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,21 +217,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -191,6 +244,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -205,6 +274,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -213,6 +312,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,41 +341,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,6 +359,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,31 +388,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,152 +548,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -492,17 +573,39 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,15 +615,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,26 +649,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -589,171 +663,214 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -808,6 +925,74 @@
     <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0092D050"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1073,17 +1258,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
-    <col min="3" max="4" width="32.625" customWidth="1"/>
+    <col min="1" max="1" width="15.8" customWidth="1"/>
+    <col min="2" max="2" width="14.8133333333333" customWidth="1"/>
+    <col min="3" max="3" width="32.62" customWidth="1"/>
+    <col min="4" max="4" width="52.7266666666667" customWidth="1"/>
+    <col min="5" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1185,7 +1375,7 @@
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="3"/>
@@ -1201,92 +1391,144 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="B22" s="6"/>
+      <c r="C22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" ht="31.5" spans="1:4">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="D23" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D10">
+  <autoFilter ref="A1:D22">
     <extLst/>
   </autoFilter>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B19:B22"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722222222222" footer="0.509722222222222"/>
+  <pageSetup paperSize="9" scale="84" firstPageNumber="0" fitToHeight="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finish lession making mp3
</commit_message>
<xml_diff>
--- a/CSS library.xlsx
+++ b/CSS library.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23175" windowHeight="9675" tabRatio="500"/>
+    <workbookView windowWidth="27795" windowHeight="12450" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$44</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>Type</t>
   </si>
@@ -220,6 +220,99 @@
   </si>
   <si>
     <t>xuống hàng -- margin có đủ</t>
+  </si>
+  <si>
+    <t>flexbox</t>
+  </si>
+  <si>
+    <t>display</t>
+  </si>
+  <si>
+    <t>flex</t>
+  </si>
+  <si>
+    <t>khi dùng flexbox thì phải khai báo flex</t>
+  </si>
+  <si>
+    <t>flex-direction</t>
+  </si>
+  <si>
+    <t>row/column</t>
+  </si>
+  <si>
+    <t>justify-content</t>
+  </si>
+  <si>
+    <t>flex-start*</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> flex-end </t>
+  </si>
+  <si>
+    <t>rigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> center</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> space-between</t>
+  </si>
+  <si>
+    <t>chia đều các chữ(không có đầu đuôi)</t>
+  </si>
+  <si>
+    <t>space-around</t>
+  </si>
+  <si>
+    <t>chia đều các chữ  (đầu = 1/2 giữa = đuôi)</t>
+  </si>
+  <si>
+    <t>space-evenly</t>
+  </si>
+  <si>
+    <t>chia đều các chữ  (đầu = giữa = đuôi)</t>
+  </si>
+  <si>
+    <t>align-items</t>
+  </si>
+  <si>
+    <t>làm theo chiều vuông góc với flex-direction</t>
+  </si>
+  <si>
+    <t>flex-basis</t>
+  </si>
+  <si>
+    <t>&lt;length&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tăng kích thước </t>
+  </si>
+  <si>
+    <t>flex-grow</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chia khoảng trống còn lại cho các phần tử </t>
+  </si>
+  <si>
+    <t>flex-shrink</t>
+  </si>
+  <si>
+    <t>1* | &lt;number&gt;</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sắp xếp </t>
   </si>
 </sst>
 </file>
@@ -227,10 +320,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -247,6 +340,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -255,9 +361,64 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -275,6 +436,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -282,126 +495,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -418,61 +511,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +679,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,116 +695,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -664,6 +757,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -678,17 +817,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,186 +867,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -920,12 +1026,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -935,11 +1050,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1330,18 +1451,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="A30:D31 C32"/>
+      <selection activeCell="B34" sqref="B34:B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="15.8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8166666666667" customWidth="1"/>
-    <col min="3" max="3" width="32.6166666666667" customWidth="1"/>
-    <col min="4" max="4" width="61.875" customWidth="1"/>
+    <col min="2" max="2" width="14.8133333333333" customWidth="1"/>
+    <col min="3" max="3" width="46.8" customWidth="1"/>
+    <col min="4" max="4" width="61.8733333333333" customWidth="1"/>
     <col min="5" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1532,10 +1653,10 @@
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1546,8 +1667,8 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="4" t="s">
         <v>41</v>
       </c>
@@ -1556,8 +1677,8 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="4" t="s">
         <v>43</v>
       </c>
@@ -1566,8 +1687,8 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="4" t="s">
         <v>45</v>
       </c>
@@ -1575,113 +1696,241 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" ht="30" spans="1:4">
-      <c r="A23" s="3"/>
+    <row r="23" ht="31.5" spans="1:4">
+      <c r="A23" s="10"/>
       <c r="B23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="11" t="s">
         <v>48</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="9" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="9"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12" t="s">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="16"/>
+      <c r="C35" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="16"/>
+      <c r="C36" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="16"/>
+      <c r="C37" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="16"/>
+      <c r="C38" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="17"/>
+      <c r="C39" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D29">
+  <autoFilter ref="A1:D44">
     <extLst/>
   </autoFilter>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A23"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B34:B39"/>
     <mergeCell ref="D28:D29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722222222222" footer="0.509722222222222"/>

</xml_diff>

<commit_message>
update css last lesson
</commit_message>
<xml_diff>
--- a/CSS library.xlsx
+++ b/CSS library.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12450" tabRatio="500"/>
+    <workbookView windowWidth="20775" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$49</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="113">
   <si>
     <t>Type</t>
   </si>
@@ -313,6 +313,51 @@
   </si>
   <si>
     <t xml:space="preserve">sắp xếp </t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>static*</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>top, left, right, bottom (vị trí tương đối so với vị trí hiện tại)</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>vị trí tương đối so với màn hình (làm nút chat , nút trở về home....)</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>giá trị tuyệt đối theo thẻ cha có thuộc tính postion : relative</t>
+  </si>
+  <si>
+    <t>sticky</t>
+  </si>
+  <si>
+    <t>2D transform</t>
+  </si>
+  <si>
+    <t>translate</t>
+  </si>
+  <si>
+    <t>rolate</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>matrix</t>
   </si>
 </sst>
 </file>
@@ -320,9 +365,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;\ _₫_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
@@ -340,6 +385,109 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -348,14 +496,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,133 +540,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -517,181 +562,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,11 +815,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,11 +860,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,47 +895,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -872,154 +917,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1027,40 +1078,43 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1451,476 +1505,568 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B39"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="15.8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8133333333333" customWidth="1"/>
+    <col min="2" max="2" width="14.8133333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="46.8" customWidth="1"/>
     <col min="4" max="4" width="61.8733333333333" customWidth="1"/>
     <col min="5" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="4" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="4" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" ht="31.5" spans="1:4">
-      <c r="A23" s="10"/>
-      <c r="B23" s="4" t="s">
+      <c r="A23" s="12"/>
+      <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="13" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="12" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="12"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="14"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="13" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="15" t="s">
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="14"/>
+      <c r="B34" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="16"/>
-      <c r="C35" s="13" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" s="14"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="16"/>
-      <c r="C36" s="13" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="14"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="16"/>
-      <c r="C37" s="13" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="14"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="2:4">
-      <c r="B38" s="16"/>
-      <c r="C38" s="13" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="14"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
-      <c r="B39" s="17"/>
-      <c r="C39" s="13" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="14"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
-      <c r="B40" s="13" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="13" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
-      <c r="B42" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
-      <c r="B43" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" t="s">
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="14"/>
+      <c r="B44" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="s">
         <v>97</v>
       </c>
     </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="20"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D44">
+  <autoFilter ref="A1:D49">
     <extLst/>
   </autoFilter>
-  <mergeCells count="11">
+  <mergeCells count="14">
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A15"/>
@@ -1928,9 +2074,12 @@
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A44"/>
+    <mergeCell ref="A45:A49"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B34:B39"/>
+    <mergeCell ref="B45:B49"/>
     <mergeCell ref="D28:D29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509722222222222" footer="0.509722222222222"/>

</xml_diff>

<commit_message>
add meta to  use media query in chrome
</commit_message>
<xml_diff>
--- a/CSS library.xlsx
+++ b/CSS library.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="133">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -649,10 +649,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+      <selection pane="topLeft" activeCell="C70" activeCellId="1" sqref="C64 C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1299,12 +1299,17 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
         <v>131</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>